<commit_message>
Scripting DPLKINV001-006 until DPLKINV001-008
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-006 - Setup Jenis Broker Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-006 - Setup Jenis Broker Investasi - General Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46C8EF3-20E3-4169-A425-E3A3A734C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3FD579-923E-4776-BFB7-A80D9AF93FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -28,9 +28,6 @@
     <t>SIDEBAR_SUBMENU</t>
   </si>
   <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
-  <si>
     <t>RUN</t>
   </si>
   <si>
@@ -52,30 +49,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>TEXT1</t>
-  </si>
-  <si>
-    <t>TEXT2</t>
-  </si>
-  <si>
-    <t>TEXT3</t>
-  </si>
-  <si>
-    <t>TEXT4</t>
-  </si>
-  <si>
-    <t>TEXT5</t>
-  </si>
-  <si>
-    <t>TEXT6</t>
-  </si>
-  <si>
-    <t>TEXT7</t>
-  </si>
-  <si>
-    <t>TEXT8</t>
-  </si>
-  <si>
     <t>Normal - Investasi - General</t>
   </si>
   <si>
@@ -104,12 +77,6 @@
   </si>
   <si>
     <t>Hapus Data Dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>TEXT9</t>
-  </si>
-  <si>
-    <t>TEXT10</t>
   </si>
   <si>
     <t>INV001-006</t>
@@ -147,6 +114,33 @@
     <t>Username : Putri;
 Password : bni1234/;
 Nama Jenis Broker : Keuangan Utama</t>
+  </si>
+  <si>
+    <t>KODE_JENIS_BROKER</t>
+  </si>
+  <si>
+    <t>NAMA_JENIS_BROKER</t>
+  </si>
+  <si>
+    <t>STATUS_REGISTER</t>
+  </si>
+  <si>
+    <t>KETERANGAN_REGISTER</t>
+  </si>
+  <si>
+    <t>KU</t>
+  </si>
+  <si>
+    <t>Keuangan</t>
+  </si>
+  <si>
+    <t>Keuangan Utama</t>
+  </si>
+  <si>
+    <t>0 : Pending Register</t>
+  </si>
+  <si>
+    <t>Testing Add Setup Jenis Broker</t>
   </si>
 </sst>
 </file>
@@ -539,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,45 +551,45 @@
     <col min="9" max="9" width="17.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="16" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="12" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="12" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>0</v>
@@ -604,228 +598,225 @@
         <v>1</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="7"/>
+      <c r="L2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
     </row>
-    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="7"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="7"/>
+      <c r="L4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
+      <c r="T4" s="4"/>
       <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
     </row>
-    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
+      <c r="T5" s="4"/>
       <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>

</xml_diff>